<commit_message>
Added End to End scenarios. Updated excel test data
</commit_message>
<xml_diff>
--- a/Resources/Data/testData.xlsx
+++ b/Resources/Data/testData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simranraina\eclipse-workspace\RestAssuredTest\src\main\java\com\rest\test\RestAssuredTest\screenshot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AAD9139B-253A-4F0E-8226-AF8181B87CB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{770F6C98-CA82-489B-9A65-F002ACE3D75E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="testdata" sheetId="1" r:id="rId1"/>
-    <sheet name="postdataUser" sheetId="2" r:id="rId2"/>
+    <sheet name="getData" sheetId="1" r:id="rId1"/>
+    <sheet name="postData" sheetId="2" r:id="rId2"/>
+    <sheet name="e2eData" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t>Id</t>
   </si>
@@ -106,6 +107,53 @@
   </si>
   <si>
     <t>This is test</t>
+  </si>
+  <si>
+    <t>TCs</t>
+  </si>
+  <si>
+    <t>uri</t>
+  </si>
+  <si>
+    <t>contenttype</t>
+  </si>
+  <si>
+    <t>request</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>/books</t>
+  </si>
+  <si>
+    <t>application/json</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>{_x000D_
+    "author": "Test Name 3",_x000D_
+    "isbn": 103,_x000D_
+    "name": "Test Book 3",_x000D_
+    "price": 999                          }</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>{_x000D_
+    "author": "New Name",_x000D_
+    "isbn": 103,_x000D_
+    "name": "New Name",_x000D_
+    "price": 999                          }</t>
+  </si>
+  <si>
+    <t>DELETE</t>
   </si>
 </sst>
 </file>
@@ -152,10 +200,14 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -497,7 +549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -638,4 +690,95 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{276D63D8-A8B9-4B14-94FA-5CA2B3E7FA5F}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="105">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="90">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>